<commit_message>
alteração nas primeiras funções
</commit_message>
<xml_diff>
--- a/ALIS_planilha_teste.xlsx
+++ b/ALIS_planilha_teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/alisonao_al_insper_edu_br/Documents/Insper/2023.2/Ciência de Dados/C.DadosP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{B0E6468A-5387-4D2E-8129-68733E097DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{256DD6AB-6E85-4BFF-A934-DFD7F37AEE79}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{B0E6468A-5387-4D2E-8129-68733E097DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D328FCC6-8A02-44F7-84C7-5D38A4FFDE3D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     <t>Comprei dois livros e os dois vieram super amassados, um na parte de baixo, e  outro na parte de cima, não só a capa, as folhas também.</t>
   </si>
   <si>
-    <t>$!#!@!# á´s~eã Para quem gosta de poemas simples, esse é o livro ideal! A autora nos faz refletir sobre alguns elementos comuns na vida das mulheres de um jeito bem leve</t>
+    <t>$!#!@!# á´s~eã Para quem gosta de poemas simples, esse é o livro ideal! A autora nos faz refletir sobre alguns                  elementos comuns na vida das mulheres de um jeito bem leve</t>
   </si>
 </sst>
 </file>
@@ -137,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,9 +147,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,7 +431,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +449,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">

</xml_diff>